<commit_message>
Update documentation, add MCM Awards, add img.
</commit_message>
<xml_diff>
--- a/documentation/套磁情况表.xlsx
+++ b/documentation/套磁情况表.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20532\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20532\CLionProjects\tochusc\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC122209-FE23-4CA6-B52A-EB80D78C534D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828B9075-45A2-4E1D-9A77-EF211DE1B835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>电子科技大学</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -79,6 +79,18 @@
   </si>
   <si>
     <t>陈洪</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>吉林大学</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>宋姗姗</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>同意开具推荐信、保留名额</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -407,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -468,29 +480,43 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
         <v>4</v>
       </c>
       <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
         <v>7</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>